<commit_message>
sesión 2025-12-14: v3.51 soporte retención IRPF alquileres
</commit_message>
<xml_diff>
--- a/src/migracion/outputs/Facturas_1T25.xlsx
+++ b/src/migracion/outputs/Facturas_1T25.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5241" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5241" uniqueCount="962">
   <si>
     <t>#</t>
   </si>
@@ -2897,9 +2897,6 @@
   </si>
   <si>
     <t>DESCUADRE: -54.11€</t>
-  </si>
-  <si>
-    <t>DESCUADRE: -95.00€</t>
   </si>
   <si>
     <t>DESCUADRE: +59.22€</t>
@@ -20987,7 +20984,7 @@
         <v>510</v>
       </c>
       <c r="J612" t="s">
-        <v>961</v>
+        <v>952</v>
       </c>
     </row>
     <row r="613" spans="1:10">
@@ -21016,7 +21013,7 @@
         <v>510</v>
       </c>
       <c r="J613" t="s">
-        <v>961</v>
+        <v>952</v>
       </c>
     </row>
     <row r="614" spans="1:10">
@@ -21551,7 +21548,7 @@
         <v>510</v>
       </c>
       <c r="J630" t="s">
-        <v>961</v>
+        <v>952</v>
       </c>
     </row>
     <row r="631" spans="1:10">
@@ -21676,7 +21673,7 @@
         <v>510</v>
       </c>
       <c r="J634" t="s">
-        <v>961</v>
+        <v>952</v>
       </c>
     </row>
     <row r="635" spans="1:10">
@@ -22455,7 +22452,7 @@
         <v>510</v>
       </c>
       <c r="J659" t="s">
-        <v>961</v>
+        <v>952</v>
       </c>
     </row>
     <row r="660" spans="1:10">
@@ -22580,7 +22577,7 @@
         <v>510</v>
       </c>
       <c r="J663" t="s">
-        <v>961</v>
+        <v>952</v>
       </c>
     </row>
     <row r="664" spans="1:10">
@@ -25048,7 +25045,7 @@
         <v>75.06999999999999</v>
       </c>
       <c r="J742" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="743" spans="1:10">

</xml_diff>